<commit_message>
Update get a version of excel reader working. Need to refactor this more.
</commit_message>
<xml_diff>
--- a/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Excel/Data/TestExcel.xlsx
+++ b/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Excel/Data/TestExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatthewB\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\personal\ExpensifyImporter\src\ExpensifyImporter\Tests\ExpensifyImporter.UnitTests\Modules\Excel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7328B01F-54FF-4AA9-8940-57FD93766B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2C4BB4-5A66-43A7-8229-D257C7DF84FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="9510" xr2:uid="{4571ACE3-4DDE-43C7-BFE1-A9885E1C2345}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{4571ACE3-4DDE-43C7-BFE1-A9885E1C2345}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Id</t>
   </si>
@@ -54,6 +52,15 @@
   </si>
   <si>
     <t>Barry</t>
+  </si>
+  <si>
+    <t>8BC78143-9FD5-45E4-AEED-F5648D58473C</t>
+  </si>
+  <si>
+    <t>46C6F115-B719-48BF-8EE1-3ABF480DF748</t>
+  </si>
+  <si>
+    <t>5088AB6B-CFCE-4531-BDFE-1E79CCAA7A3D</t>
   </si>
 </sst>
 </file>
@@ -408,12 +415,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="39.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,9 +434,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -435,9 +445,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -446,9 +456,9 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -459,5 +469,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>